<commit_message>
More colleges input into database
</commit_message>
<xml_diff>
--- a/smartgrid/dbdata/Spreadsheets/Colleges.xlsx
+++ b/smartgrid/dbdata/Spreadsheets/Colleges.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="28060" yWindow="-6340" windowWidth="15180" windowHeight="14960" tabRatio="500"/>
+    <workbookView xWindow="25860" yWindow="-6760" windowWidth="15180" windowHeight="14960" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="24">
   <si>
     <t>UC Berkeley Extension</t>
   </si>
@@ -52,13 +52,52 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>UC Davis</t>
+  </si>
+  <si>
+    <t>Certification Program in Green Building and Sustainable Design</t>
+  </si>
+  <si>
+    <t>UC Berkeley Seminars</t>
+  </si>
+  <si>
+    <t>Certificate Program in Energy Resource Management</t>
+  </si>
+  <si>
+    <t>Certificate Program in Renewable Energy</t>
+  </si>
+  <si>
+    <t>Professional Concentration in Solar Energy Systems and Design</t>
+  </si>
+  <si>
+    <t>Mechanical Engineering</t>
+  </si>
+  <si>
+    <t>Electrical Engineering</t>
+  </si>
+  <si>
+    <t>Computer Science</t>
+  </si>
+  <si>
+    <t>Environment Resources Sciences</t>
+  </si>
+  <si>
+    <t>UC Irvine</t>
+  </si>
+  <si>
+    <t>Sustainable Business Management</t>
+  </si>
+  <si>
+    <t>Others</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -70,6 +109,22 @@
       <sz val="13"/>
       <color rgb="FF000000"/>
       <name val="Helvetica"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -89,14 +144,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="5">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -426,10 +489,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -474,10 +537,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="D3" t="s">
         <v>10</v>
@@ -494,7 +554,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D4" t="s">
         <v>10</v>
@@ -511,7 +571,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D5" t="s">
         <v>10</v>
@@ -528,7 +588,7 @@
         <v>3</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D6" t="s">
         <v>10</v>
@@ -545,17 +605,25 @@
         <v>3</v>
       </c>
       <c r="C7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="C8" s="1"/>
       <c r="D8" t="s">
         <v>10</v>
       </c>
@@ -564,12 +632,253 @@
       </c>
     </row>
     <row r="9" spans="1:5">
+      <c r="A9">
+        <v>9</v>
+      </c>
+      <c r="B9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="D9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10">
+        <v>10</v>
+      </c>
+      <c r="B10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11">
+        <v>11</v>
+      </c>
+      <c r="B11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12">
+        <v>12</v>
+      </c>
+      <c r="B12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13">
+        <v>13</v>
+      </c>
+      <c r="B13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14">
+        <v>14</v>
+      </c>
+      <c r="B14" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15">
+        <v>15</v>
+      </c>
+      <c r="B15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D15" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16">
+        <v>16</v>
+      </c>
+      <c r="B16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D16" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17">
+        <v>17</v>
+      </c>
+      <c r="B17" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D17" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18">
+        <v>18</v>
+      </c>
+      <c r="B18" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D18" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19">
+        <v>19</v>
+      </c>
+      <c r="B19" t="s">
+        <v>21</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D19" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20">
+        <v>20</v>
+      </c>
+      <c r="B20" t="s">
+        <v>21</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D20" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21">
+        <v>21</v>
+      </c>
+      <c r="B21" t="s">
+        <v>21</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D21" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="D22" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="D23" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="D24" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="D25" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="D26" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="D27" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="D28" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="D29" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="D30" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="D31" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="D32" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33" spans="4:4">
+      <c r="D33" t="s">
         <v>10</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
UCLA / Irvine / Modified Colleges
</commit_message>
<xml_diff>
--- a/smartgrid/dbdata/Spreadsheets/Colleges.xlsx
+++ b/smartgrid/dbdata/Spreadsheets/Colleges.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="29">
   <si>
     <t>UC Berkeley Extension</t>
   </si>
@@ -91,6 +91,21 @@
   </si>
   <si>
     <t>Others</t>
+  </si>
+  <si>
+    <t>UCLA</t>
+  </si>
+  <si>
+    <t>Plumbing Systems Design</t>
+  </si>
+  <si>
+    <t>Sequential Program in HVAC Design</t>
+  </si>
+  <si>
+    <t>Southern</t>
+  </si>
+  <si>
+    <t>Certificate in Global Sustainability</t>
   </si>
 </sst>
 </file>
@@ -492,7 +507,7 @@
   <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -661,6 +676,9 @@
       <c r="D10" t="s">
         <v>10</v>
       </c>
+      <c r="E10" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11">
@@ -675,6 +693,9 @@
       <c r="D11" t="s">
         <v>10</v>
       </c>
+      <c r="E11" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12">
@@ -689,6 +710,9 @@
       <c r="D12" t="s">
         <v>10</v>
       </c>
+      <c r="E12" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13">
@@ -703,6 +727,9 @@
       <c r="D13" t="s">
         <v>10</v>
       </c>
+      <c r="E13" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14">
@@ -717,6 +744,9 @@
       <c r="D14" t="s">
         <v>10</v>
       </c>
+      <c r="E14" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15">
@@ -731,6 +761,9 @@
       <c r="D15" t="s">
         <v>10</v>
       </c>
+      <c r="E15" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16">
@@ -745,8 +778,11 @@
       <c r="D16" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="17" spans="1:4">
+      <c r="E16" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
       <c r="A17">
         <v>17</v>
       </c>
@@ -759,8 +795,11 @@
       <c r="D17" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="18" spans="1:4">
+      <c r="E17" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
       <c r="A18">
         <v>18</v>
       </c>
@@ -773,8 +812,11 @@
       <c r="D18" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="19" spans="1:4">
+      <c r="E18" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
       <c r="A19">
         <v>19</v>
       </c>
@@ -787,8 +829,11 @@
       <c r="D19" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="20" spans="1:4">
+      <c r="E19" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
       <c r="A20">
         <v>20</v>
       </c>
@@ -801,8 +846,11 @@
       <c r="D20" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="21" spans="1:4">
+      <c r="E20" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
       <c r="A21">
         <v>21</v>
       </c>
@@ -815,58 +863,130 @@
       <c r="D21" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="22" spans="1:4">
+      <c r="E21" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22">
+        <v>22</v>
+      </c>
+      <c r="B22" t="s">
+        <v>24</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>25</v>
+      </c>
       <c r="D22" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="23" spans="1:4">
+      <c r="E22" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23">
+        <v>23</v>
+      </c>
+      <c r="B23" t="s">
+        <v>24</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="D23" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="24" spans="1:4">
+      <c r="E23" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24">
+        <v>24</v>
+      </c>
+      <c r="B24" t="s">
+        <v>24</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="D24" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:5">
+      <c r="A25">
+        <v>25</v>
+      </c>
+      <c r="B25" t="s">
+        <v>24</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="D25" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:5">
+      <c r="A26">
+        <v>26</v>
+      </c>
+      <c r="B26" t="s">
+        <v>24</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="D26" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:5">
+      <c r="A27">
+        <v>27</v>
+      </c>
+      <c r="B27" t="s">
+        <v>24</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="D27" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:5">
+      <c r="A28">
+        <v>28</v>
+      </c>
+      <c r="B28" t="s">
+        <v>24</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>23</v>
+      </c>
       <c r="D28" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:5">
       <c r="D29" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:5">
       <c r="D30" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:5">
       <c r="D31" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:5">
       <c r="D32" t="s">
         <v>10</v>
       </c>

</xml_diff>

<commit_message>
Added in headers for reference
</commit_message>
<xml_diff>
--- a/smartgrid/dbdata/Spreadsheets/Colleges.xlsx
+++ b/smartgrid/dbdata/Spreadsheets/Colleges.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="25860" yWindow="-6760" windowWidth="15180" windowHeight="14960" tabRatio="500"/>
+    <workbookView xWindow="25860" yWindow="-6765" windowWidth="15180" windowHeight="11760" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="50">
   <si>
     <t>UC Berkeley Extension</t>
   </si>
@@ -154,6 +154,21 @@
   </si>
   <si>
     <t>Computer Engineering</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Degree</t>
+  </si>
+  <si>
+    <t>Site</t>
+  </si>
+  <si>
+    <t>Region</t>
   </si>
 </sst>
 </file>
@@ -252,6 +267,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -577,42 +597,47 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E55"/>
+  <dimension ref="A1:E56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="D64" sqref="D64"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="5" width="21.6640625" customWidth="1"/>
+    <col min="1" max="2" width="21.625" customWidth="1"/>
+    <col min="3" max="3" width="30.125" customWidth="1"/>
+    <col min="4" max="4" width="47.25" customWidth="1"/>
+    <col min="5" max="5" width="21.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1">
-        <v>1</v>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>45</v>
       </c>
       <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>7</v>
+        <v>46</v>
+      </c>
+      <c r="C1" t="s">
+        <v>47</v>
       </c>
       <c r="D1" t="s">
-        <v>2</v>
+        <v>48</v>
       </c>
       <c r="E1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="1"/>
+      <c r="C2" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="D2" t="s">
         <v>2</v>
       </c>
@@ -620,13 +645,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="C3" s="1"/>
       <c r="D3" t="s">
         <v>2</v>
       </c>
@@ -634,66 +660,63 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A5">
         <v>4</v>
-      </c>
-      <c r="B4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5">
-        <v>5</v>
       </c>
       <c r="B5" t="s">
         <v>3</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A6">
         <v>5</v>
-      </c>
-      <c r="D5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6">
-        <v>6</v>
       </c>
       <c r="B6" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A7">
         <v>6</v>
-      </c>
-      <c r="D6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7">
-        <v>7</v>
       </c>
       <c r="B7" t="s">
         <v>3</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D7" t="s">
         <v>10</v>
@@ -702,49 +725,49 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8" t="s">
         <v>3</v>
       </c>
       <c r="C8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9">
+      <c r="D9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A10">
         <v>9</v>
-      </c>
-      <c r="B9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9" t="s">
-        <v>10</v>
-      </c>
-      <c r="E9" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10">
-        <v>10</v>
       </c>
       <c r="B10" t="s">
         <v>11</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D10" t="s">
         <v>10</v>
@@ -753,15 +776,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11" t="s">
         <v>11</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D11" t="s">
         <v>10</v>
@@ -770,15 +793,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B12" t="s">
         <v>11</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D12" t="s">
         <v>10</v>
@@ -787,15 +810,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B13" t="s">
         <v>11</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D13" t="s">
         <v>10</v>
@@ -804,15 +827,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B14" t="s">
         <v>11</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D14" t="s">
         <v>10</v>
@@ -821,15 +844,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B15" t="s">
         <v>11</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D15" t="s">
         <v>10</v>
@@ -838,49 +861,49 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B16" t="s">
         <v>11</v>
       </c>
       <c r="C16" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" t="s">
+        <v>10</v>
+      </c>
+      <c r="E16" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>11</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D16" t="s">
-        <v>10</v>
-      </c>
-      <c r="E16" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="A17">
+      <c r="D17" t="s">
+        <v>10</v>
+      </c>
+      <c r="E17" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A18">
         <v>17</v>
-      </c>
-      <c r="B17" t="s">
-        <v>21</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D17" t="s">
-        <v>10</v>
-      </c>
-      <c r="E17" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
-      <c r="A18">
-        <v>18</v>
       </c>
       <c r="B18" t="s">
         <v>21</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="D18" t="s">
         <v>10</v>
@@ -889,15 +912,15 @@
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B19" t="s">
         <v>21</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D19" t="s">
         <v>10</v>
@@ -906,15 +929,15 @@
         <v>27</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B20" t="s">
         <v>21</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D20" t="s">
         <v>10</v>
@@ -923,49 +946,49 @@
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B21" t="s">
         <v>21</v>
       </c>
       <c r="C21" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D21" t="s">
+        <v>10</v>
+      </c>
+      <c r="E21" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>21</v>
+      </c>
+      <c r="C22" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D21" t="s">
-        <v>10</v>
-      </c>
-      <c r="E21" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5">
-      <c r="A22">
+      <c r="D22" t="s">
+        <v>10</v>
+      </c>
+      <c r="E22" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A23">
         <v>22</v>
-      </c>
-      <c r="B22" t="s">
-        <v>24</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D22" t="s">
-        <v>10</v>
-      </c>
-      <c r="E22" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5">
-      <c r="A23">
-        <v>23</v>
       </c>
       <c r="B23" t="s">
         <v>24</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D23" t="s">
         <v>10</v>
@@ -974,15 +997,15 @@
         <v>27</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B24" t="s">
         <v>24</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D24" t="s">
         <v>10</v>
@@ -991,15 +1014,15 @@
         <v>27</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B25" t="s">
         <v>24</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="D25" t="s">
         <v>10</v>
@@ -1008,15 +1031,15 @@
         <v>27</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B26" t="s">
         <v>24</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D26" t="s">
         <v>10</v>
@@ -1025,15 +1048,15 @@
         <v>27</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B27" t="s">
         <v>24</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D27" t="s">
         <v>10</v>
@@ -1042,49 +1065,49 @@
         <v>27</v>
       </c>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B28" t="s">
         <v>24</v>
       </c>
       <c r="C28" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D28" t="s">
+        <v>10</v>
+      </c>
+      <c r="E28" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>24</v>
+      </c>
+      <c r="C29" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D28" t="s">
-        <v>10</v>
-      </c>
-      <c r="E28" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5">
-      <c r="A29">
+      <c r="D29" t="s">
+        <v>10</v>
+      </c>
+      <c r="E29" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A30">
         <v>29</v>
-      </c>
-      <c r="B29" t="s">
-        <v>29</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D29" t="s">
-        <v>30</v>
-      </c>
-      <c r="E29" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5">
-      <c r="A30">
-        <v>30</v>
       </c>
       <c r="B30" t="s">
         <v>29</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D30" t="s">
         <v>30</v>
@@ -1093,15 +1116,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:5">
+    <row r="31" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B31" t="s">
         <v>29</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D31" t="s">
         <v>30</v>
@@ -1110,15 +1133,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B32" t="s">
         <v>29</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="D32" t="s">
         <v>30</v>
@@ -1127,32 +1150,32 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
+        <v>29</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D33" t="s">
+        <v>30</v>
+      </c>
+      <c r="E33" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A34">
         <v>33</v>
-      </c>
-      <c r="B33" t="s">
-        <v>32</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D33" t="s">
-        <v>37</v>
-      </c>
-      <c r="E33" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5">
-      <c r="A34">
-        <v>34</v>
       </c>
       <c r="B34" t="s">
         <v>32</v>
       </c>
-      <c r="C34" s="2" t="s">
-        <v>34</v>
+      <c r="C34" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="D34" t="s">
         <v>37</v>
@@ -1161,15 +1184,15 @@
         <v>27</v>
       </c>
     </row>
-    <row r="35" spans="1:5">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B35" t="s">
         <v>32</v>
       </c>
-      <c r="C35" s="3" t="s">
-        <v>35</v>
+      <c r="C35" s="2" t="s">
+        <v>34</v>
       </c>
       <c r="D35" t="s">
         <v>37</v>
@@ -1178,15 +1201,15 @@
         <v>27</v>
       </c>
     </row>
-    <row r="36" spans="1:5">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B36" t="s">
         <v>32</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D36" t="s">
         <v>37</v>
@@ -1195,15 +1218,15 @@
         <v>27</v>
       </c>
     </row>
-    <row r="37" spans="1:5">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B37" t="s">
         <v>32</v>
       </c>
-      <c r="C37" t="s">
-        <v>17</v>
+      <c r="C37" s="3" t="s">
+        <v>36</v>
       </c>
       <c r="D37" t="s">
         <v>37</v>
@@ -1212,15 +1235,15 @@
         <v>27</v>
       </c>
     </row>
-    <row r="38" spans="1:5">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B38" t="s">
         <v>32</v>
       </c>
       <c r="C38" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D38" t="s">
         <v>37</v>
@@ -1229,15 +1252,15 @@
         <v>27</v>
       </c>
     </row>
-    <row r="39" spans="1:5">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B39" t="s">
         <v>32</v>
       </c>
       <c r="C39" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D39" t="s">
         <v>37</v>
@@ -1246,15 +1269,15 @@
         <v>27</v>
       </c>
     </row>
-    <row r="40" spans="1:5">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B40" t="s">
         <v>32</v>
       </c>
       <c r="C40" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D40" t="s">
         <v>37</v>
@@ -1263,213 +1286,230 @@
         <v>27</v>
       </c>
     </row>
-    <row r="41" spans="1:5">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41" t="s">
+        <v>32</v>
+      </c>
+      <c r="C41" t="s">
+        <v>23</v>
+      </c>
+      <c r="D41" t="s">
+        <v>37</v>
+      </c>
+      <c r="E41" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42">
         <v>41</v>
-      </c>
-      <c r="B41" t="s">
-        <v>38</v>
-      </c>
-      <c r="C41" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="E41" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5">
-      <c r="A42">
-        <v>42</v>
       </c>
       <c r="B42" t="s">
         <v>38</v>
       </c>
-      <c r="C42" t="s">
-        <v>40</v>
+      <c r="C42" s="4" t="s">
+        <v>39</v>
       </c>
       <c r="E42" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="43" spans="1:5">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B43" t="s">
         <v>38</v>
       </c>
       <c r="C43" t="s">
-        <v>17</v>
+        <v>40</v>
       </c>
       <c r="E43" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="44" spans="1:5">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B44" t="s">
         <v>38</v>
       </c>
       <c r="C44" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E44" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="45" spans="1:5">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B45" t="s">
         <v>38</v>
       </c>
       <c r="C45" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E45" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="46" spans="1:5">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B46" t="s">
         <v>38</v>
       </c>
       <c r="C46" t="s">
+        <v>19</v>
+      </c>
+      <c r="E46" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>46</v>
+      </c>
+      <c r="B47" t="s">
+        <v>38</v>
+      </c>
+      <c r="C47" t="s">
         <v>23</v>
       </c>
-      <c r="E46" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5">
-      <c r="A47">
+      <c r="E47" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48">
         <v>47</v>
-      </c>
-      <c r="B47" t="s">
-        <v>41</v>
-      </c>
-      <c r="C47" t="s">
-        <v>42</v>
-      </c>
-      <c r="E47" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5">
-      <c r="A48">
-        <v>48</v>
       </c>
       <c r="B48" t="s">
         <v>41</v>
       </c>
       <c r="C48" t="s">
-        <v>17</v>
+        <v>42</v>
       </c>
       <c r="E48" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="49" spans="1:5">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B49" t="s">
         <v>41</v>
       </c>
       <c r="C49" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E49" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="50" spans="1:5">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B50" t="s">
         <v>41</v>
       </c>
       <c r="C50" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E50" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="51" spans="1:5">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B51" t="s">
         <v>41</v>
       </c>
       <c r="C51" t="s">
+        <v>19</v>
+      </c>
+      <c r="E51" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>51</v>
+      </c>
+      <c r="B52" t="s">
+        <v>41</v>
+      </c>
+      <c r="C52" t="s">
         <v>23</v>
       </c>
-      <c r="E51" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5">
-      <c r="A52">
+      <c r="E52" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53">
         <v>52</v>
-      </c>
-      <c r="B52" t="s">
-        <v>43</v>
-      </c>
-      <c r="C52" t="s">
-        <v>18</v>
-      </c>
-      <c r="E52" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5">
-      <c r="A53">
-        <v>53</v>
       </c>
       <c r="B53" t="s">
         <v>43</v>
       </c>
       <c r="C53" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E53" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:5">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B54" t="s">
         <v>43</v>
       </c>
       <c r="C54" t="s">
-        <v>44</v>
+        <v>19</v>
       </c>
       <c r="E54" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:5">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B55" t="s">
         <v>43</v>
       </c>
       <c r="C55" t="s">
+        <v>44</v>
+      </c>
+      <c r="E55" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>55</v>
+      </c>
+      <c r="B56" t="s">
+        <v>43</v>
+      </c>
+      <c r="C56" t="s">
         <v>23</v>
       </c>
-      <c r="E55" t="s">
+      <c r="E56" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>